<commit_message>
Move from IONOS site
</commit_message>
<xml_diff>
--- a/mgatour/season21/chinney.xlsx
+++ b/mgatour/season21/chinney.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David Rouse.LAPTOP-185AKRON\Documents\Melbage\melbageweb\season21\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Documents\Melbage\melbageweb\season21\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22CBBA56-C23C-4720-8B98-5B93C4CCD33B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F6175A7-4422-44BA-872A-FC1B00CC85A6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="chinney" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -159,10 +161,10 @@
     <t>Hoppo Challenge 21/09/19</t>
   </si>
   <si>
-    <t>Thommo Classic TBA</t>
-  </si>
-  <si>
     <t>Bubble Open     28/9/19</t>
+  </si>
+  <si>
+    <t>Hoppo Challenge 5/12/20</t>
   </si>
 </sst>
 </file>
@@ -1258,21 +1260,21 @@
       <selection sqref="A1:L42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.7109375" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.140625" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" customWidth="1"/>
-    <col min="5" max="5" width="11.85546875" customWidth="1"/>
-    <col min="6" max="7" width="9.7109375" customWidth="1"/>
-    <col min="8" max="8" width="11.5703125" customWidth="1"/>
-    <col min="9" max="9" width="9.42578125" customWidth="1"/>
+    <col min="1" max="1" width="8.6640625" customWidth="1"/>
+    <col min="2" max="2" width="17.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.109375" customWidth="1"/>
+    <col min="4" max="4" width="10.33203125" customWidth="1"/>
+    <col min="5" max="5" width="11.88671875" customWidth="1"/>
+    <col min="6" max="7" width="9.6640625" customWidth="1"/>
+    <col min="8" max="8" width="11.5546875" customWidth="1"/>
+    <col min="9" max="9" width="9.44140625" customWidth="1"/>
     <col min="10" max="10" width="10" customWidth="1"/>
-    <col min="11" max="12" width="10.28515625" customWidth="1"/>
+    <col min="11" max="12" width="10.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2"/>
       <c r="B1" s="12" t="s">
         <v>36</v>
@@ -1288,7 +1290,7 @@
       <c r="K1" s="12"/>
       <c r="L1" s="2"/>
     </row>
-    <row r="2" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2"/>
       <c r="B2" s="12"/>
       <c r="C2" s="12"/>
@@ -1302,7 +1304,7 @@
       <c r="K2" s="12"/>
       <c r="L2" s="2"/>
     </row>
-    <row r="3" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
       <c r="B3" s="13" t="s">
         <v>0</v>
@@ -1318,7 +1320,7 @@
       <c r="K3" s="13"/>
       <c r="L3" s="2"/>
     </row>
-    <row r="4" spans="1:12" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2"/>
       <c r="B4" s="3"/>
       <c r="C4" s="4" t="s">
@@ -1331,7 +1333,7 @@
         <v>39</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G4" s="5" t="s">
         <v>40</v>
@@ -1343,14 +1345,14 @@
         <v>42</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="K4" s="6" t="s">
         <v>1</v>
       </c>
       <c r="L4" s="2"/>
     </row>
-    <row r="5" spans="1:12" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2"/>
       <c r="B5" s="14" t="s">
         <v>2</v>
@@ -1366,7 +1368,7 @@
       <c r="K5" s="16"/>
       <c r="L5" s="2"/>
     </row>
-    <row r="6" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2"/>
       <c r="B6" s="8" t="s">
         <v>5</v>
@@ -1375,143 +1377,153 @@
       <c r="D6" s="9">
         <v>36</v>
       </c>
-      <c r="E6" s="9">
-        <v>25</v>
-      </c>
+      <c r="E6" s="9"/>
       <c r="F6" s="9">
         <v>33</v>
       </c>
-      <c r="G6" s="9"/>
+      <c r="G6" s="9">
+        <v>25</v>
+      </c>
       <c r="H6" s="9">
         <v>19</v>
       </c>
       <c r="I6" s="9">
         <v>0</v>
       </c>
-      <c r="J6" s="9"/>
+      <c r="J6" s="9">
+        <v>27</v>
+      </c>
       <c r="K6" s="10">
         <f>SUM(C6:J6)</f>
-        <v>113</v>
+        <v>140</v>
       </c>
       <c r="L6" s="2"/>
     </row>
-    <row r="7" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2"/>
       <c r="B7" s="8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C7" s="9"/>
       <c r="D7" s="9">
+        <v>40</v>
+      </c>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9">
+        <v>0</v>
+      </c>
+      <c r="G7" s="9">
         <v>32</v>
       </c>
-      <c r="E7" s="9">
-        <v>34</v>
-      </c>
-      <c r="F7" s="9">
-        <v>34</v>
-      </c>
-      <c r="G7" s="9"/>
       <c r="H7" s="9">
         <v>0</v>
       </c>
       <c r="I7" s="9">
-        <v>0</v>
-      </c>
-      <c r="J7" s="9"/>
+        <v>22</v>
+      </c>
+      <c r="J7" s="9">
+        <v>31</v>
+      </c>
       <c r="K7" s="10">
         <f>SUM(C7:J7)</f>
-        <v>100</v>
+        <v>125</v>
       </c>
       <c r="L7" s="2"/>
     </row>
-    <row r="8" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2"/>
       <c r="B8" s="8" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="C8" s="9"/>
       <c r="D8" s="9">
-        <v>26</v>
-      </c>
-      <c r="E8" s="9">
-        <v>38</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="E8" s="9"/>
       <c r="F8" s="9">
-        <v>0</v>
-      </c>
-      <c r="G8" s="9"/>
+        <v>29</v>
+      </c>
+      <c r="G8" s="9">
+        <v>0</v>
+      </c>
       <c r="H8" s="9">
+        <v>0</v>
+      </c>
+      <c r="I8" s="9">
+        <v>23</v>
+      </c>
+      <c r="J8" s="9">
         <v>32</v>
       </c>
-      <c r="I8" s="9">
-        <v>0</v>
-      </c>
-      <c r="J8" s="9"/>
       <c r="K8" s="10">
         <f>SUM(C8:J8)</f>
-        <v>96</v>
+        <v>116</v>
       </c>
       <c r="L8" s="2"/>
     </row>
-    <row r="9" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2"/>
       <c r="B9" s="8" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C9" s="9"/>
       <c r="D9" s="9">
-        <v>40</v>
-      </c>
-      <c r="E9" s="9">
         <v>32</v>
       </c>
+      <c r="E9" s="9"/>
       <c r="F9" s="9">
-        <v>0</v>
-      </c>
-      <c r="G9" s="9"/>
+        <v>34</v>
+      </c>
+      <c r="G9" s="9">
+        <v>34</v>
+      </c>
       <c r="H9" s="9">
         <v>0</v>
       </c>
       <c r="I9" s="9">
-        <v>22</v>
-      </c>
-      <c r="J9" s="9"/>
+        <v>0</v>
+      </c>
+      <c r="J9" s="9">
+        <v>0</v>
+      </c>
       <c r="K9" s="10">
         <f>SUM(C9:J9)</f>
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="L9" s="2"/>
     </row>
-    <row r="10" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2"/>
       <c r="B10" s="8" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C10" s="9"/>
       <c r="D10" s="9">
+        <v>26</v>
+      </c>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9">
+        <v>0</v>
+      </c>
+      <c r="G10" s="9">
+        <v>38</v>
+      </c>
+      <c r="H10" s="9">
         <v>32</v>
       </c>
-      <c r="E10" s="9">
-        <v>0</v>
-      </c>
-      <c r="F10" s="9">
-        <v>29</v>
-      </c>
-      <c r="G10" s="9"/>
-      <c r="H10" s="9">
-        <v>0</v>
-      </c>
       <c r="I10" s="9">
-        <v>23</v>
-      </c>
-      <c r="J10" s="9"/>
+        <v>0</v>
+      </c>
+      <c r="J10" s="9">
+        <v>0</v>
+      </c>
       <c r="K10" s="10">
         <f>SUM(C10:J10)</f>
-        <v>84</v>
+        <v>96</v>
       </c>
       <c r="L10" s="2"/>
     </row>
-    <row r="11" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2"/>
       <c r="B11" s="8" t="s">
         <v>7</v>
@@ -1520,85 +1532,91 @@
       <c r="D11" s="9">
         <v>22</v>
       </c>
-      <c r="E11" s="9">
+      <c r="E11" s="9"/>
+      <c r="F11" s="9">
+        <v>0</v>
+      </c>
+      <c r="G11" s="9">
         <v>25</v>
       </c>
-      <c r="F11" s="9">
-        <v>0</v>
-      </c>
-      <c r="G11" s="9"/>
       <c r="H11" s="9">
         <v>30</v>
       </c>
       <c r="I11" s="9">
         <v>0</v>
       </c>
-      <c r="J11" s="9"/>
+      <c r="J11" s="9">
+        <v>18</v>
+      </c>
       <c r="K11" s="10">
         <f>SUM(C11:J11)</f>
-        <v>77</v>
+        <v>95</v>
       </c>
       <c r="L11" s="2"/>
     </row>
-    <row r="12" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2"/>
       <c r="B12" s="8" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C12" s="9"/>
       <c r="D12" s="9">
-        <v>31</v>
-      </c>
-      <c r="E12" s="9">
         <v>32</v>
       </c>
+      <c r="E12" s="9"/>
       <c r="F12" s="9">
         <v>0</v>
       </c>
-      <c r="G12" s="9"/>
+      <c r="G12" s="9">
+        <v>0</v>
+      </c>
       <c r="H12" s="9">
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="I12" s="9">
         <v>0</v>
       </c>
-      <c r="J12" s="9"/>
+      <c r="J12" s="9">
+        <v>34</v>
+      </c>
       <c r="K12" s="10">
         <f>SUM(C12:J12)</f>
-        <v>63</v>
+        <v>95</v>
       </c>
       <c r="L12" s="2"/>
     </row>
-    <row r="13" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2"/>
       <c r="B13" s="8" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C13" s="9"/>
       <c r="D13" s="9">
+        <v>31</v>
+      </c>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9">
+        <v>0</v>
+      </c>
+      <c r="G13" s="9">
         <v>32</v>
       </c>
-      <c r="E13" s="9">
-        <v>0</v>
-      </c>
-      <c r="F13" s="9">
-        <v>0</v>
-      </c>
-      <c r="G13" s="9"/>
       <c r="H13" s="9">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="I13" s="9">
         <v>0</v>
       </c>
-      <c r="J13" s="9"/>
+      <c r="J13" s="9">
+        <v>0</v>
+      </c>
       <c r="K13" s="10">
         <f>SUM(C13:J13)</f>
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="L13" s="2"/>
     </row>
-    <row r="14" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2"/>
       <c r="B14" s="8" t="s">
         <v>14</v>
@@ -1607,27 +1625,29 @@
       <c r="D14" s="9">
         <v>0</v>
       </c>
-      <c r="E14" s="9">
-        <v>23</v>
-      </c>
+      <c r="E14" s="9"/>
       <c r="F14" s="9">
         <v>37</v>
       </c>
-      <c r="G14" s="9"/>
+      <c r="G14" s="9">
+        <v>23</v>
+      </c>
       <c r="H14" s="9">
         <v>0</v>
       </c>
       <c r="I14" s="9">
         <v>0</v>
       </c>
-      <c r="J14" s="9"/>
+      <c r="J14" s="9">
+        <v>0</v>
+      </c>
       <c r="K14" s="10">
         <f>SUM(C14:J14)</f>
         <v>60</v>
       </c>
       <c r="L14" s="2"/>
     </row>
-    <row r="15" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2"/>
       <c r="B15" s="8" t="s">
         <v>9</v>
@@ -1636,27 +1656,29 @@
       <c r="D15" s="9">
         <v>40</v>
       </c>
-      <c r="E15" s="9">
-        <v>0</v>
-      </c>
+      <c r="E15" s="9"/>
       <c r="F15" s="9">
         <v>0</v>
       </c>
-      <c r="G15" s="9"/>
+      <c r="G15" s="9">
+        <v>0</v>
+      </c>
       <c r="H15" s="9">
         <v>19</v>
       </c>
       <c r="I15" s="9">
         <v>0</v>
       </c>
-      <c r="J15" s="9"/>
+      <c r="J15" s="9">
+        <v>0</v>
+      </c>
       <c r="K15" s="10">
         <f>SUM(C15:J15)</f>
         <v>59</v>
       </c>
       <c r="L15" s="2"/>
     </row>
-    <row r="16" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2"/>
       <c r="B16" s="8" t="s">
         <v>10</v>
@@ -1665,27 +1687,29 @@
       <c r="D16" s="9">
         <v>0</v>
       </c>
-      <c r="E16" s="9">
-        <v>0</v>
-      </c>
+      <c r="E16" s="9"/>
       <c r="F16" s="9">
         <v>0</v>
       </c>
-      <c r="G16" s="9"/>
+      <c r="G16" s="9">
+        <v>0</v>
+      </c>
       <c r="H16" s="9">
         <v>31</v>
       </c>
       <c r="I16" s="9">
         <v>0</v>
       </c>
-      <c r="J16" s="9"/>
+      <c r="J16" s="9">
+        <v>0</v>
+      </c>
       <c r="K16" s="10">
         <f>SUM(C16:J16)</f>
         <v>31</v>
       </c>
       <c r="L16" s="2"/>
     </row>
-    <row r="17" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2"/>
       <c r="B17" s="8" t="s">
         <v>11</v>
@@ -1694,27 +1718,29 @@
       <c r="D17" s="9">
         <v>0</v>
       </c>
-      <c r="E17" s="9">
-        <v>0</v>
-      </c>
+      <c r="E17" s="9"/>
       <c r="F17" s="9">
         <v>0</v>
       </c>
-      <c r="G17" s="9"/>
+      <c r="G17" s="9">
+        <v>0</v>
+      </c>
       <c r="H17" s="9">
         <v>0</v>
       </c>
       <c r="I17" s="9">
         <v>0</v>
       </c>
-      <c r="J17" s="9"/>
+      <c r="J17" s="9">
+        <v>0</v>
+      </c>
       <c r="K17" s="10">
         <f>SUM(C17:J17)</f>
         <v>0</v>
       </c>
       <c r="L17" s="2"/>
     </row>
-    <row r="18" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2"/>
       <c r="B18" s="8" t="s">
         <v>13</v>
@@ -1723,27 +1749,29 @@
       <c r="D18" s="9">
         <v>0</v>
       </c>
-      <c r="E18" s="9">
-        <v>0</v>
-      </c>
+      <c r="E18" s="9"/>
       <c r="F18" s="9">
         <v>0</v>
       </c>
-      <c r="G18" s="9"/>
+      <c r="G18" s="9">
+        <v>0</v>
+      </c>
       <c r="H18" s="9">
         <v>0</v>
       </c>
       <c r="I18" s="9">
         <v>0</v>
       </c>
-      <c r="J18" s="9"/>
+      <c r="J18" s="9">
+        <v>0</v>
+      </c>
       <c r="K18" s="10">
         <f>SUM(C18:J18)</f>
         <v>0</v>
       </c>
       <c r="L18" s="2"/>
     </row>
-    <row r="19" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2"/>
       <c r="B19" s="8" t="s">
         <v>15</v>
@@ -1752,27 +1780,29 @@
       <c r="D19" s="9">
         <v>0</v>
       </c>
-      <c r="E19" s="9">
-        <v>0</v>
-      </c>
+      <c r="E19" s="9"/>
       <c r="F19" s="9">
         <v>0</v>
       </c>
-      <c r="G19" s="9"/>
+      <c r="G19" s="9">
+        <v>0</v>
+      </c>
       <c r="H19" s="9">
         <v>0</v>
       </c>
       <c r="I19" s="9">
         <v>0</v>
       </c>
-      <c r="J19" s="9"/>
+      <c r="J19" s="9">
+        <v>0</v>
+      </c>
       <c r="K19" s="10">
         <f>SUM(C19:J19)</f>
         <v>0</v>
       </c>
       <c r="L19" s="2"/>
     </row>
-    <row r="20" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2"/>
       <c r="B20" s="8" t="s">
         <v>17</v>
@@ -1781,27 +1811,29 @@
       <c r="D20" s="9">
         <v>0</v>
       </c>
-      <c r="E20" s="9">
-        <v>0</v>
-      </c>
+      <c r="E20" s="9"/>
       <c r="F20" s="9">
         <v>0</v>
       </c>
-      <c r="G20" s="9"/>
+      <c r="G20" s="9">
+        <v>0</v>
+      </c>
       <c r="H20" s="9">
         <v>0</v>
       </c>
       <c r="I20" s="9">
         <v>0</v>
       </c>
-      <c r="J20" s="9"/>
+      <c r="J20" s="9">
+        <v>0</v>
+      </c>
       <c r="K20" s="10">
         <f>SUM(C20:J20)</f>
         <v>0</v>
       </c>
       <c r="L20" s="2"/>
     </row>
-    <row r="21" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2"/>
       <c r="B21" s="8" t="s">
         <v>18</v>
@@ -1810,27 +1842,29 @@
       <c r="D21" s="9">
         <v>0</v>
       </c>
-      <c r="E21" s="9">
-        <v>0</v>
-      </c>
+      <c r="E21" s="9"/>
       <c r="F21" s="9">
         <v>0</v>
       </c>
-      <c r="G21" s="9"/>
+      <c r="G21" s="9">
+        <v>0</v>
+      </c>
       <c r="H21" s="9">
         <v>0</v>
       </c>
       <c r="I21" s="9">
         <v>0</v>
       </c>
-      <c r="J21" s="9"/>
+      <c r="J21" s="9">
+        <v>0</v>
+      </c>
       <c r="K21" s="10">
         <f>SUM(C21:J21)</f>
         <v>0</v>
       </c>
       <c r="L21" s="2"/>
     </row>
-    <row r="22" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2"/>
       <c r="B22" s="7"/>
       <c r="C22" s="10">
@@ -1843,7 +1877,7 @@
       </c>
       <c r="E22" s="10">
         <f t="shared" si="0"/>
-        <v>209</v>
+        <v>0</v>
       </c>
       <c r="F22" s="10">
         <f t="shared" si="0"/>
@@ -1851,7 +1885,7 @@
       </c>
       <c r="G22" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>209</v>
       </c>
       <c r="H22" s="10">
         <f t="shared" si="0"/>
@@ -1863,15 +1897,15 @@
       </c>
       <c r="J22" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>142</v>
       </c>
       <c r="K22" s="10">
         <f t="shared" ref="K22" si="1">SUM(C22:J22)</f>
-        <v>838</v>
+        <v>980</v>
       </c>
       <c r="L22" s="2"/>
     </row>
-    <row r="23" spans="1:12" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2"/>
       <c r="B23" s="17" t="s">
         <v>19</v>
@@ -1887,7 +1921,7 @@
       <c r="K23" s="19"/>
       <c r="L23" s="2"/>
     </row>
-    <row r="24" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2"/>
       <c r="B24" s="8" t="s">
         <v>21</v>
@@ -1896,27 +1930,29 @@
       <c r="D24" s="9">
         <v>33</v>
       </c>
-      <c r="E24" s="9">
-        <v>35</v>
-      </c>
+      <c r="E24" s="9"/>
       <c r="F24" s="9">
         <v>29</v>
       </c>
-      <c r="G24" s="9"/>
+      <c r="G24" s="9">
+        <v>35</v>
+      </c>
       <c r="H24" s="9">
         <v>31</v>
       </c>
       <c r="I24" s="9">
         <v>23</v>
       </c>
-      <c r="J24" s="9"/>
+      <c r="J24" s="9">
+        <v>31</v>
+      </c>
       <c r="K24" s="10">
         <f>SUM(C24:J24)</f>
-        <v>151</v>
+        <v>182</v>
       </c>
       <c r="L24" s="2"/>
     </row>
-    <row r="25" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2"/>
       <c r="B25" s="8" t="s">
         <v>20</v>
@@ -1925,27 +1961,29 @@
       <c r="D25" s="9">
         <v>38</v>
       </c>
-      <c r="E25" s="9">
-        <v>22</v>
-      </c>
+      <c r="E25" s="9"/>
       <c r="F25" s="9">
         <v>31</v>
       </c>
-      <c r="G25" s="9"/>
+      <c r="G25" s="9">
+        <v>22</v>
+      </c>
       <c r="H25" s="9">
         <v>25</v>
       </c>
       <c r="I25" s="9">
         <v>33</v>
       </c>
-      <c r="J25" s="9"/>
+      <c r="J25" s="9">
+        <v>0</v>
+      </c>
       <c r="K25" s="10">
         <f>SUM(C25:J25)</f>
         <v>149</v>
       </c>
       <c r="L25" s="2"/>
     </row>
-    <row r="26" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2"/>
       <c r="B26" s="8" t="s">
         <v>22</v>
@@ -1954,27 +1992,29 @@
       <c r="D26" s="9">
         <v>32</v>
       </c>
-      <c r="E26" s="9">
-        <v>31</v>
-      </c>
+      <c r="E26" s="9"/>
       <c r="F26" s="9">
         <v>26</v>
       </c>
-      <c r="G26" s="9"/>
+      <c r="G26" s="9">
+        <v>31</v>
+      </c>
       <c r="H26" s="9">
         <v>0</v>
       </c>
       <c r="I26" s="9">
         <v>25</v>
       </c>
-      <c r="J26" s="9"/>
+      <c r="J26" s="9">
+        <v>31</v>
+      </c>
       <c r="K26" s="10">
         <f>SUM(C26:J26)</f>
-        <v>114</v>
+        <v>145</v>
       </c>
       <c r="L26" s="2"/>
     </row>
-    <row r="27" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="2"/>
       <c r="B27" s="8" t="s">
         <v>25</v>
@@ -1983,288 +2023,308 @@
       <c r="D27" s="9">
         <v>0</v>
       </c>
-      <c r="E27" s="9">
-        <v>0</v>
-      </c>
+      <c r="E27" s="9"/>
       <c r="F27" s="9">
         <v>33</v>
       </c>
-      <c r="G27" s="9"/>
+      <c r="G27" s="9">
+        <v>0</v>
+      </c>
       <c r="H27" s="9">
         <v>34</v>
       </c>
       <c r="I27" s="9">
         <v>0</v>
       </c>
-      <c r="J27" s="9"/>
+      <c r="J27" s="9">
+        <v>0</v>
+      </c>
       <c r="K27" s="10">
         <f>SUM(C27:J27)</f>
         <v>67</v>
       </c>
       <c r="L27" s="2"/>
     </row>
-    <row r="28" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="2"/>
       <c r="B28" s="8" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="C28" s="9"/>
       <c r="D28" s="9">
         <v>0</v>
       </c>
-      <c r="E28" s="9">
-        <v>29</v>
-      </c>
+      <c r="E28" s="9"/>
       <c r="F28" s="9">
         <v>0</v>
       </c>
-      <c r="G28" s="9"/>
+      <c r="G28" s="9">
+        <v>0</v>
+      </c>
       <c r="H28" s="9">
         <v>0</v>
       </c>
       <c r="I28" s="9">
-        <v>26</v>
-      </c>
-      <c r="J28" s="9"/>
+        <v>24</v>
+      </c>
+      <c r="J28" s="9">
+        <v>32</v>
+      </c>
       <c r="K28" s="10">
         <f>SUM(C28:J28)</f>
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="L28" s="2"/>
     </row>
-    <row r="29" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="2"/>
       <c r="B29" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C29" s="9"/>
       <c r="D29" s="9">
         <v>0</v>
       </c>
-      <c r="E29" s="9">
-        <v>34</v>
-      </c>
+      <c r="E29" s="9"/>
       <c r="F29" s="9">
         <v>0</v>
       </c>
-      <c r="G29" s="9"/>
+      <c r="G29" s="9">
+        <v>29</v>
+      </c>
       <c r="H29" s="9">
         <v>0</v>
       </c>
       <c r="I29" s="9">
-        <v>0</v>
-      </c>
-      <c r="J29" s="9"/>
+        <v>26</v>
+      </c>
+      <c r="J29" s="9">
+        <v>0</v>
+      </c>
       <c r="K29" s="10">
         <f>SUM(C29:J29)</f>
-        <v>34</v>
+        <v>55</v>
       </c>
       <c r="L29" s="2"/>
     </row>
-    <row r="30" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="2"/>
       <c r="B30" s="8" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C30" s="9"/>
       <c r="D30" s="9">
         <v>0</v>
       </c>
-      <c r="E30" s="9">
-        <v>0</v>
-      </c>
+      <c r="E30" s="9"/>
       <c r="F30" s="9">
-        <v>26</v>
-      </c>
-      <c r="G30" s="9"/>
+        <v>24</v>
+      </c>
+      <c r="G30" s="9">
+        <v>0</v>
+      </c>
       <c r="H30" s="9">
         <v>0</v>
       </c>
       <c r="I30" s="9">
         <v>0</v>
       </c>
-      <c r="J30" s="9"/>
+      <c r="J30" s="9">
+        <v>27</v>
+      </c>
       <c r="K30" s="10">
         <f>SUM(C30:J30)</f>
-        <v>26</v>
+        <v>51</v>
       </c>
       <c r="L30" s="2"/>
     </row>
-    <row r="31" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="2"/>
       <c r="B31" s="8" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C31" s="9"/>
       <c r="D31" s="9">
         <v>0</v>
       </c>
-      <c r="E31" s="9">
-        <v>0</v>
-      </c>
+      <c r="E31" s="9"/>
       <c r="F31" s="9">
         <v>0</v>
       </c>
-      <c r="G31" s="9"/>
+      <c r="G31" s="9">
+        <v>34</v>
+      </c>
       <c r="H31" s="9">
         <v>0</v>
       </c>
       <c r="I31" s="9">
-        <v>25</v>
-      </c>
-      <c r="J31" s="9"/>
+        <v>0</v>
+      </c>
+      <c r="J31" s="9">
+        <v>0</v>
+      </c>
       <c r="K31" s="10">
         <f>SUM(C31:J31)</f>
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="L31" s="2"/>
     </row>
-    <row r="32" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="2"/>
       <c r="B32" s="8" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C32" s="9"/>
       <c r="D32" s="9">
         <v>0</v>
       </c>
-      <c r="E32" s="9">
-        <v>0</v>
-      </c>
+      <c r="E32" s="9"/>
       <c r="F32" s="9">
-        <v>0</v>
-      </c>
-      <c r="G32" s="9"/>
+        <v>26</v>
+      </c>
+      <c r="G32" s="9">
+        <v>0</v>
+      </c>
       <c r="H32" s="9">
         <v>0</v>
       </c>
       <c r="I32" s="9">
-        <v>24</v>
-      </c>
-      <c r="J32" s="9"/>
+        <v>0</v>
+      </c>
+      <c r="J32" s="9">
+        <v>0</v>
+      </c>
       <c r="K32" s="10">
         <f>SUM(C32:J32)</f>
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="L32" s="2"/>
     </row>
-    <row r="33" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="2"/>
       <c r="B33" s="8" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C33" s="9"/>
       <c r="D33" s="9">
         <v>0</v>
       </c>
-      <c r="E33" s="9">
-        <v>0</v>
-      </c>
+      <c r="E33" s="9"/>
       <c r="F33" s="9">
-        <v>24</v>
-      </c>
-      <c r="G33" s="9"/>
+        <v>0</v>
+      </c>
+      <c r="G33" s="9">
+        <v>0</v>
+      </c>
       <c r="H33" s="9">
         <v>0</v>
       </c>
       <c r="I33" s="9">
-        <v>0</v>
-      </c>
-      <c r="J33" s="9"/>
+        <v>25</v>
+      </c>
+      <c r="J33" s="9">
+        <v>0</v>
+      </c>
       <c r="K33" s="10">
         <f>SUM(C33:J33)</f>
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L33" s="2"/>
     </row>
-    <row r="34" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="2"/>
       <c r="B34" s="8" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="C34" s="9"/>
       <c r="D34" s="9">
         <v>0</v>
       </c>
-      <c r="E34" s="9">
-        <v>0</v>
-      </c>
+      <c r="E34" s="9"/>
       <c r="F34" s="9">
         <v>0</v>
       </c>
-      <c r="G34" s="9"/>
+      <c r="G34" s="9">
+        <v>0</v>
+      </c>
       <c r="H34" s="9">
         <v>0</v>
       </c>
       <c r="I34" s="9">
         <v>0</v>
       </c>
-      <c r="J34" s="9"/>
+      <c r="J34" s="9">
+        <v>25</v>
+      </c>
       <c r="K34" s="10">
         <f>SUM(C34:J34)</f>
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="L34" s="2"/>
     </row>
-    <row r="35" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="2"/>
       <c r="B35" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C35" s="9"/>
       <c r="D35" s="9">
         <v>0</v>
       </c>
-      <c r="E35" s="9">
-        <v>0</v>
-      </c>
+      <c r="E35" s="9"/>
       <c r="F35" s="9">
         <v>0</v>
       </c>
-      <c r="G35" s="9"/>
+      <c r="G35" s="9">
+        <v>0</v>
+      </c>
       <c r="H35" s="9">
         <v>0</v>
       </c>
       <c r="I35" s="9">
         <v>0</v>
       </c>
-      <c r="J35" s="9"/>
+      <c r="J35" s="9">
+        <v>0</v>
+      </c>
       <c r="K35" s="10">
         <f>SUM(C35:J35)</f>
         <v>0</v>
       </c>
       <c r="L35" s="2"/>
     </row>
-    <row r="36" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="2"/>
       <c r="B36" s="8" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C36" s="9"/>
       <c r="D36" s="9">
         <v>0</v>
       </c>
-      <c r="E36" s="9">
-        <v>0</v>
-      </c>
+      <c r="E36" s="9"/>
       <c r="F36" s="9">
         <v>0</v>
       </c>
-      <c r="G36" s="9"/>
+      <c r="G36" s="9">
+        <v>0</v>
+      </c>
       <c r="H36" s="9">
         <v>0</v>
       </c>
       <c r="I36" s="9">
         <v>0</v>
       </c>
-      <c r="J36" s="9"/>
+      <c r="J36" s="9">
+        <v>0</v>
+      </c>
       <c r="K36" s="10">
         <f>SUM(C36:J36)</f>
         <v>0</v>
       </c>
       <c r="L36" s="2"/>
     </row>
-    <row r="37" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="2"/>
       <c r="B37" s="8" t="s">
         <v>33</v>
@@ -2273,27 +2333,29 @@
       <c r="D37" s="9">
         <v>0</v>
       </c>
-      <c r="E37" s="9">
-        <v>0</v>
-      </c>
+      <c r="E37" s="9"/>
       <c r="F37" s="9">
         <v>0</v>
       </c>
-      <c r="G37" s="9"/>
+      <c r="G37" s="9">
+        <v>0</v>
+      </c>
       <c r="H37" s="9">
         <v>0</v>
       </c>
       <c r="I37" s="9">
         <v>0</v>
       </c>
-      <c r="J37" s="9"/>
+      <c r="J37" s="9">
+        <v>0</v>
+      </c>
       <c r="K37" s="10">
         <f>SUM(C37:J37)</f>
         <v>0</v>
       </c>
       <c r="L37" s="2"/>
     </row>
-    <row r="38" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="2"/>
       <c r="B38" s="8" t="s">
         <v>34</v>
@@ -2302,27 +2364,29 @@
       <c r="D38" s="9">
         <v>0</v>
       </c>
-      <c r="E38" s="9">
-        <v>0</v>
-      </c>
+      <c r="E38" s="9"/>
       <c r="F38" s="9">
         <v>0</v>
       </c>
-      <c r="G38" s="9"/>
+      <c r="G38" s="9">
+        <v>0</v>
+      </c>
       <c r="H38" s="9">
         <v>0</v>
       </c>
       <c r="I38" s="9">
         <v>0</v>
       </c>
-      <c r="J38" s="9"/>
+      <c r="J38" s="9">
+        <v>0</v>
+      </c>
       <c r="K38" s="10">
         <f>SUM(C38:J38)</f>
         <v>0</v>
       </c>
       <c r="L38" s="2"/>
     </row>
-    <row r="39" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="2"/>
       <c r="B39" s="8" t="s">
         <v>35</v>
@@ -2331,27 +2395,29 @@
       <c r="D39" s="9">
         <v>0</v>
       </c>
-      <c r="E39" s="9">
-        <v>0</v>
-      </c>
+      <c r="E39" s="9"/>
       <c r="F39" s="9">
         <v>0</v>
       </c>
-      <c r="G39" s="9"/>
+      <c r="G39" s="9">
+        <v>0</v>
+      </c>
       <c r="H39" s="9">
         <v>0</v>
       </c>
       <c r="I39" s="9">
         <v>0</v>
       </c>
-      <c r="J39" s="9"/>
+      <c r="J39" s="9">
+        <v>0</v>
+      </c>
       <c r="K39" s="10">
         <f>SUM(C39:J39)</f>
         <v>0</v>
       </c>
       <c r="L39" s="2"/>
     </row>
-    <row r="40" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="2"/>
       <c r="B40" s="7"/>
       <c r="C40" s="10">
@@ -2364,7 +2430,7 @@
       </c>
       <c r="E40" s="10">
         <f t="shared" si="2"/>
-        <v>151</v>
+        <v>0</v>
       </c>
       <c r="F40" s="10">
         <f t="shared" si="2"/>
@@ -2372,7 +2438,7 @@
       </c>
       <c r="G40" s="10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>151</v>
       </c>
       <c r="H40" s="10">
         <f t="shared" si="2"/>
@@ -2384,15 +2450,15 @@
       </c>
       <c r="J40" s="10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>146</v>
       </c>
       <c r="K40" s="10">
         <f t="shared" si="2"/>
-        <v>669</v>
+        <v>815</v>
       </c>
       <c r="L40" s="2"/>
     </row>
-    <row r="41" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="2"/>
       <c r="B41" s="11"/>
       <c r="C41" s="2"/>
@@ -2406,7 +2472,7 @@
       <c r="K41" s="2"/>
       <c r="L41" s="2"/>
     </row>
-    <row r="42" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="2"/>
       <c r="B42" s="11"/>
       <c r="C42" s="2"/>
@@ -2433,7 +2499,7 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing r:id="rId1"/>
   <webPublishItems count="1">
-    <webPublishItem id="1900" divId="chinney_1900" sourceType="range" sourceRef="A1:L42" destinationFile="C:\Users\David Rouse.LAPTOP-185AKRON\Documents\Melbage\melbageweb\season21\chinney.htm"/>
+    <webPublishItem id="1900" divId="chinney_1900" sourceType="range" sourceRef="A1:L42" destinationFile="C:\Users\david\Documents\Melbage\melbageweb\season21\chinney.htm"/>
   </webPublishItems>
 </worksheet>
 </file>
</xml_diff>